<commit_message>
Fixed some points of the schematic
</commit_message>
<xml_diff>
--- a/doc/2230_TubePitotDeporte-JOURNAL_v1.0.0.xlsx
+++ b/doc/2230_TubePitotDeporte-JOURNAL_v1.0.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mevricchier\OneDrive - Education Vaud\2ndYear\PROJ\2230_TubePitotDeporte\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mevricchier\Documents\2230_TubePitotDeporte\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,21 @@
   </si>
   <si>
     <t>Création du projet Altium et début du schéma électrique avec dimentionnement des composants</t>
+  </si>
+  <si>
+    <t>Dimentionnement et choix de composants et design du schéma électriques</t>
+  </si>
+  <si>
+    <t>Dimanche</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport et design du schéma électrique</t>
+  </si>
+  <si>
+    <t>Mardi</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport et corrections du schéma électrique</t>
   </si>
 </sst>
 </file>
@@ -507,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:E19"/>
+  <dimension ref="B5:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,16 +720,76 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="6"/>
+      <c r="B18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="14">
+        <v>44579</v>
+      </c>
+      <c r="D18" s="8">
+        <v>8</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="13">
+        <v>44583</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="14">
+        <v>44585</v>
+      </c>
+      <c r="D20" s="8">
+        <v>4</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
PCB done, BOM not ready
</commit_message>
<xml_diff>
--- a/doc/2230_TubePitotDeporte-JOURNAL_v1.0.0.xlsx
+++ b/doc/2230_TubePitotDeporte-JOURNAL_v1.0.0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\School\PROJ\2230_TubePitotDeporte\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mevricchier\Documents\2230_TubePitotDeporte\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5674688B-BC87-4509-9483-8452AF315A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="12975"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -121,12 +120,15 @@
   </si>
   <si>
     <t xml:space="preserve">Placement des composants et routage du PCB </t>
+  </si>
+  <si>
+    <t>Routage du PCB, contrôle du PCB par Ali Zoubir et modification de la BOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -546,23 +548,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:E33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.265625" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" style="1"/>
-    <col min="3" max="3" width="11.265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="154.73046875" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="154.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
@@ -576,7 +578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -590,7 +592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
@@ -604,7 +606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -618,7 +620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
@@ -632,7 +634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
@@ -646,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -660,7 +662,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
@@ -674,7 +676,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -688,7 +690,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -702,7 +704,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
@@ -716,7 +718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
@@ -730,7 +732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -744,7 +746,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>9</v>
       </c>
@@ -758,7 +760,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
@@ -772,7 +774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>22</v>
       </c>
@@ -786,7 +788,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -800,7 +802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>10</v>
       </c>
@@ -814,7 +816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
@@ -828,7 +830,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>9</v>
       </c>
@@ -842,7 +844,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>10</v>
       </c>
@@ -856,7 +858,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>9</v>
       </c>
@@ -870,7 +872,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>9</v>
       </c>
@@ -884,7 +886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>22</v>
       </c>
@@ -898,7 +900,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -912,7 +914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>10</v>
       </c>
@@ -926,23 +928,75 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B32" s="8"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="13">
+        <v>44996</v>
+      </c>
+      <c r="D31" s="4">
+        <v>4</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="14">
+        <v>45000</v>
+      </c>
+      <c r="D32" s="8">
+        <v>8</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>